<commit_message>
changed how to read datasets
</commit_message>
<xml_diff>
--- a/Datasets/RawDatasets/Costo orario risorse - budget.xlsx
+++ b/Datasets/RawDatasets/Costo orario risorse - budget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SCGProject/Datasets/RawDatasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58045A9-75E8-A74B-9B05-2FBBA36D34CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D7EE4-929D-9F4A-96A6-347673282C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,10 +115,10 @@
     <t>Risorsa</t>
   </si>
   <si>
-    <t>AreaProduzione</t>
-  </si>
-  <si>
-    <t>CostoOrario</t>
+    <t>Area di produzione</t>
+  </si>
+  <si>
+    <t>Costo orario (€/h)</t>
   </si>
 </sst>
 </file>
@@ -514,14 +514,14 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added tables for scostamento
</commit_message>
<xml_diff>
--- a/Datasets/RawDatasets/Costo orario risorse - budget.xlsx
+++ b/Datasets/RawDatasets/Costo orario risorse - budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcovinciguerra/Github/SCGProject/Datasets/RawDatasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D7EE4-929D-9F4A-96A6-347673282C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A50D7F-72C6-1F44-A8CD-BAF432F0B4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>